<commit_message>
Shop & Summon System Update
상점 및 소환 시스템 업데이트
기존 CashTable 파일 내용이 변경되었습니다
</commit_message>
<xml_diff>
--- a/GameDesign/데이터 테이블/CashTable.xlsx
+++ b/GameDesign/데이터 테이블/CashTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github_Project\Team_Pearl\GameDesign\데이터 테이블\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B868CA05-8307-47A3-AB8C-81DAE62208FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A37FC07-F1B2-4934-9774-4C87A9FA7D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13860" yWindow="2640" windowWidth="18045" windowHeight="11385" xr2:uid="{B1BBAB8F-C173-4CA1-8DA8-3A69E87C63C6}"/>
+    <workbookView xWindow="-28920" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{B1BBAB8F-C173-4CA1-8DA8-3A69E87C63C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>ProductID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -98,6 +98,53 @@
   </si>
   <si>
     <t>ItemID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>크리스탈 100개</t>
+  </si>
+  <si>
+    <t>Crystal_100</t>
+  </si>
+  <si>
+    <t>크리스탈 100개 묶음</t>
+  </si>
+  <si>
+    <t>크리스탈 1000개</t>
+  </si>
+  <si>
+    <t>Crystal_1000</t>
+  </si>
+  <si>
+    <t>크리스탈 1000개 묶음</t>
+  </si>
+  <si>
+    <t>크리스탈 10000개</t>
+  </si>
+  <si>
+    <t>Crystal_10000</t>
+  </si>
+  <si>
+    <t>크리스탈 10000개 묶음</t>
+  </si>
+  <si>
+    <t>크리스탈 + 골드 패키지</t>
+  </si>
+  <si>
+    <t>Crystal_Gold</t>
+  </si>
+  <si>
+    <t>크리스탈 + 마력석 패키지</t>
+  </si>
+  <si>
+    <t>Crystal_Manastone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">크리스탈 400개%n+%n2000골드 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">크리스탈 400개%n+%n100마력석 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -150,12 +197,18 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -175,9 +228,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -215,7 +268,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -321,7 +374,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -463,7 +516,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -471,25 +524,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE2C8B2-D613-49CA-8897-226459D97510}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.125" customWidth="1"/>
-    <col min="3" max="3" width="16.375" customWidth="1"/>
-    <col min="4" max="4" width="12.25" customWidth="1"/>
-    <col min="5" max="5" width="11.75" customWidth="1"/>
-    <col min="7" max="7" width="12.75" customWidth="1"/>
-    <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="10" max="10" width="12.25" customWidth="1"/>
-    <col min="11" max="11" width="12.5" customWidth="1"/>
-    <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="12.625" customWidth="1"/>
-    <col min="14" max="14" width="14.875" customWidth="1"/>
+    <col min="1" max="1" width="9" style="2"/>
+    <col min="2" max="2" width="25" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.75" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9" style="2"/>
+    <col min="7" max="7" width="12.75" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.25" style="2" customWidth="1"/>
+    <col min="11" max="11" width="12.5" style="2" customWidth="1"/>
+    <col min="12" max="12" width="17" style="2" customWidth="1"/>
+    <col min="13" max="13" width="18.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -537,6 +594,211 @@
       </c>
       <c r="O1" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1100</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <v>45373</v>
+      </c>
+      <c r="I2" s="3">
+        <v>73050</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>10000</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>45292</v>
+      </c>
+      <c r="I3" s="3">
+        <v>45372</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>99000</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>45292</v>
+      </c>
+      <c r="I4" s="3">
+        <v>45372</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4900</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>45292</v>
+      </c>
+      <c r="I5" s="3">
+        <v>45372</v>
+      </c>
+      <c r="J5" s="2">
+        <v>2</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>4900</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>45292</v>
+      </c>
+      <c r="I6" s="3">
+        <v>45372</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" s="2">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>